<commit_message>
Fixed bug in beacon creater
</commit_message>
<xml_diff>
--- a/BeaconFormat.xlsx
+++ b/BeaconFormat.xlsx
@@ -502,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9991E4-E839-4A30-B048-D2E4463FC534}">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -719,6 +719,67 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="C14">
+        <v>1820467200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>